<commit_message>
Backup QR Scanner data - 2025-08-14T07:43:59.789Z - Cache Bust: 1755157439789
</commit_message>
<xml_diff>
--- a/log_history/Y1_B2223_Anatomy_checklist1755157078081_admin@admin.com.xlsx
+++ b/log_history/Y1_B2223_Anatomy_checklist1755157078081_admin@admin.com.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,7 +424,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>232000</v>
+        <v>231249</v>
       </c>
       <c r="B2" t="str">
         <v>Anatomy</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>231999</v>
+        <v>232000</v>
       </c>
       <c r="B3" t="str">
         <v>Anatomy</v>
@@ -453,7 +453,7 @@
         <v>14/08/2025</v>
       </c>
       <c r="D3" t="str">
-        <v>10:38:03</v>
+        <v>10:38:02</v>
       </c>
       <c r="E3" t="str">
         <v>Scan</v>
@@ -464,7 +464,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>232001</v>
+        <v>231999</v>
       </c>
       <c r="B4" t="str">
         <v>Anatomy</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>235000</v>
+        <v>232001</v>
       </c>
       <c r="B5" t="str">
         <v>Anatomy</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>235010</v>
+        <v>235000</v>
       </c>
       <c r="B6" t="str">
         <v>Anatomy</v>
@@ -513,7 +513,7 @@
         <v>14/08/2025</v>
       </c>
       <c r="D6" t="str">
-        <v>10:38:05</v>
+        <v>10:38:03</v>
       </c>
       <c r="E6" t="str">
         <v>Scan</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>235020</v>
+        <v>235010</v>
       </c>
       <c r="B7" t="str">
         <v>Anatomy</v>
@@ -542,9 +542,29 @@
         <v>admin@admin.com</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>235020</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C8" t="str">
+        <v>14/08/2025</v>
+      </c>
+      <c r="D8" t="str">
+        <v>10:38:05</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F8" t="str">
+        <v>admin@admin.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>